<commit_message>
Get Draft  By Id and Get All Drafts
</commit_message>
<xml_diff>
--- a/doc/screendrafts-data.xlsx
+++ b/doc/screendrafts-data.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\ScreenDrafts.Api\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0895781E-E666-4019-87D5-043FFB63FF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89025E2C-0E86-449D-AB89-3125996B95B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="77295" yWindow="600" windowWidth="26010" windowHeight="21105" xr2:uid="{543E17E2-D959-453D-8EEC-3611A98E523F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Drafts" sheetId="1" r:id="rId1"/>
+    <sheet name="Hosts" sheetId="4" r:id="rId2"/>
+    <sheet name="Movies" sheetId="2" r:id="rId3"/>
+    <sheet name="Drafters" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3091" uniqueCount="2292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3358" uniqueCount="2301">
   <si>
     <t>Title</t>
   </si>
@@ -6913,6 +6915,33 @@
   </si>
   <si>
     <t>Frank Berman</t>
+  </si>
+  <si>
+    <t>Merchant/ Ivory</t>
+  </si>
+  <si>
+    <t>Queer Studio Movies</t>
+  </si>
+  <si>
+    <t>Rocky/ Creed Super Draft</t>
+  </si>
+  <si>
+    <t>Screwball Comedy mini-Mega</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Union Movies</t>
+  </si>
+  <si>
+    <t>Fivequels</t>
+  </si>
+  <si>
+    <t>90's Superhero</t>
+  </si>
+  <si>
+    <t>Cody Downs</t>
   </si>
 </sst>
 </file>
@@ -6948,11 +6977,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7268,10 +7296,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7B191F-AEF0-41F2-A245-FCC3CD937556}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M240"/>
+  <dimension ref="A1:M247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2:K247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7287,7 +7318,7 @@
     <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" customWidth="1"/>
     <col min="12" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -7327,7 +7358,7 @@
       <c r="L1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -7353,7 +7384,7 @@
       <c r="L2">
         <v>7</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="2">
         <v>43330</v>
       </c>
     </row>
@@ -7376,7 +7407,7 @@
       <c r="L3">
         <v>7</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="2">
         <v>43347</v>
       </c>
     </row>
@@ -7402,7 +7433,7 @@
       <c r="L4">
         <v>7</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="2">
         <v>43361</v>
       </c>
     </row>
@@ -7428,7 +7459,7 @@
       <c r="L5">
         <v>7</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="2">
         <v>43375</v>
       </c>
     </row>
@@ -7454,7 +7485,7 @@
       <c r="L6">
         <v>7</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="2">
         <v>43391</v>
       </c>
     </row>
@@ -7480,7 +7511,7 @@
       <c r="L7">
         <v>7</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="2">
         <v>43403</v>
       </c>
     </row>
@@ -7500,7 +7531,7 @@
       <c r="L8">
         <v>7</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="2">
         <v>43419</v>
       </c>
     </row>
@@ -7526,7 +7557,7 @@
       <c r="L9">
         <v>7</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="2">
         <v>43431</v>
       </c>
     </row>
@@ -7552,7 +7583,7 @@
       <c r="L10">
         <v>7</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="2">
         <v>43446</v>
       </c>
     </row>
@@ -7578,7 +7609,7 @@
       <c r="L11">
         <v>7</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="2">
         <v>43455</v>
       </c>
     </row>
@@ -7604,7 +7635,7 @@
       <c r="L12">
         <v>7</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="2">
         <v>43473</v>
       </c>
     </row>
@@ -7630,7 +7661,7 @@
       <c r="L13">
         <v>7</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="2">
         <v>43482</v>
       </c>
     </row>
@@ -7653,7 +7684,7 @@
       <c r="L14">
         <v>17</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14" s="2">
         <v>43494</v>
       </c>
     </row>
@@ -7679,7 +7710,7 @@
       <c r="L15">
         <v>7</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M15" s="2">
         <v>43508</v>
       </c>
     </row>
@@ -7705,7 +7736,7 @@
       <c r="L16">
         <v>7</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16" s="2">
         <v>43522</v>
       </c>
     </row>
@@ -7731,7 +7762,7 @@
       <c r="L17">
         <v>7</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M17" s="2">
         <v>43529</v>
       </c>
     </row>
@@ -7757,7 +7788,7 @@
       <c r="L18">
         <v>7</v>
       </c>
-      <c r="M18" s="1">
+      <c r="M18" s="2">
         <v>43537</v>
       </c>
     </row>
@@ -7777,7 +7808,7 @@
       <c r="L19">
         <v>7</v>
       </c>
-      <c r="M19" s="1">
+      <c r="M19" s="2">
         <v>43544</v>
       </c>
     </row>
@@ -7803,7 +7834,7 @@
       <c r="L20">
         <v>7</v>
       </c>
-      <c r="M20" s="1">
+      <c r="M20" s="2">
         <v>43551</v>
       </c>
     </row>
@@ -7829,7 +7860,7 @@
       <c r="L21">
         <v>7</v>
       </c>
-      <c r="M21" s="1">
+      <c r="M21" s="2">
         <v>43559</v>
       </c>
     </row>
@@ -7849,7 +7880,7 @@
       <c r="L22">
         <v>7</v>
       </c>
-      <c r="M22" s="1">
+      <c r="M22" s="2">
         <v>43570</v>
       </c>
     </row>
@@ -7875,7 +7906,7 @@
       <c r="L23">
         <v>21</v>
       </c>
-      <c r="M23" s="1">
+      <c r="M23" s="2">
         <v>43578</v>
       </c>
     </row>
@@ -7898,7 +7929,7 @@
       <c r="L24">
         <v>7</v>
       </c>
-      <c r="M24" s="1">
+      <c r="M24" s="2">
         <v>43586</v>
       </c>
     </row>
@@ -7924,7 +7955,7 @@
       <c r="L25">
         <v>7</v>
       </c>
-      <c r="M25" s="1">
+      <c r="M25" s="2">
         <v>43592</v>
       </c>
     </row>
@@ -7950,7 +7981,7 @@
       <c r="L26">
         <v>7</v>
       </c>
-      <c r="M26" s="1">
+      <c r="M26" s="2">
         <v>43599</v>
       </c>
     </row>
@@ -7976,7 +8007,7 @@
       <c r="L27">
         <v>7</v>
       </c>
-      <c r="M27" s="1">
+      <c r="M27" s="2">
         <v>43607</v>
       </c>
     </row>
@@ -8002,7 +8033,7 @@
       <c r="L28">
         <v>7</v>
       </c>
-      <c r="M28" s="1">
+      <c r="M28" s="2">
         <v>43617</v>
       </c>
     </row>
@@ -8028,7 +8059,7 @@
       <c r="L29">
         <v>7</v>
       </c>
-      <c r="M29" s="1">
+      <c r="M29" s="2">
         <v>43621</v>
       </c>
     </row>
@@ -8051,7 +8082,7 @@
       <c r="L30">
         <v>7</v>
       </c>
-      <c r="M30" s="1">
+      <c r="M30" s="2">
         <v>43628</v>
       </c>
     </row>
@@ -8077,7 +8108,7 @@
       <c r="L31">
         <v>7</v>
       </c>
-      <c r="M31" s="1">
+      <c r="M31" s="2">
         <v>43634</v>
       </c>
     </row>
@@ -8103,7 +8134,7 @@
       <c r="L32">
         <v>7</v>
       </c>
-      <c r="M32" s="1">
+      <c r="M32" s="2">
         <v>43641</v>
       </c>
     </row>
@@ -8129,7 +8160,7 @@
       <c r="L33">
         <v>7</v>
       </c>
-      <c r="M33" s="1">
+      <c r="M33" s="2">
         <v>43648</v>
       </c>
     </row>
@@ -8155,7 +8186,7 @@
       <c r="L34">
         <v>7</v>
       </c>
-      <c r="M34" s="1">
+      <c r="M34" s="2">
         <v>43655</v>
       </c>
     </row>
@@ -8181,7 +8212,7 @@
       <c r="L35">
         <v>7</v>
       </c>
-      <c r="M35" s="1">
+      <c r="M35" s="2">
         <v>43662</v>
       </c>
     </row>
@@ -8207,7 +8238,7 @@
       <c r="L36">
         <v>7</v>
       </c>
-      <c r="M36" s="1">
+      <c r="M36" s="2">
         <v>43669</v>
       </c>
     </row>
@@ -8215,7 +8246,7 @@
       <c r="A37">
         <v>37</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>436</v>
       </c>
       <c r="C37" t="s">
@@ -8230,7 +8261,7 @@
       <c r="L37">
         <v>7</v>
       </c>
-      <c r="M37" s="1">
+      <c r="M37" s="2">
         <v>43676</v>
       </c>
     </row>
@@ -8262,7 +8293,7 @@
       <c r="L38">
         <v>20</v>
       </c>
-      <c r="M38" s="1">
+      <c r="M38" s="2">
         <v>43684</v>
       </c>
     </row>
@@ -8282,7 +8313,7 @@
       <c r="L39">
         <v>7</v>
       </c>
-      <c r="M39" s="1">
+      <c r="M39" s="2">
         <v>43694</v>
       </c>
     </row>
@@ -8308,7 +8339,7 @@
       <c r="L40">
         <v>7</v>
       </c>
-      <c r="M40" t="s">
+      <c r="M40" s="2" t="s">
         <v>90</v>
       </c>
     </row>
@@ -8340,7 +8371,7 @@
       <c r="L41">
         <v>20</v>
       </c>
-      <c r="M41" s="1">
+      <c r="M41" s="2">
         <v>43704</v>
       </c>
     </row>
@@ -8363,7 +8394,7 @@
       <c r="L42">
         <v>7</v>
       </c>
-      <c r="M42" s="1">
+      <c r="M42" s="2">
         <v>43718</v>
       </c>
     </row>
@@ -8389,7 +8420,7 @@
       <c r="L43">
         <v>7</v>
       </c>
-      <c r="M43" t="s">
+      <c r="M43" s="2" t="s">
         <v>100</v>
       </c>
     </row>
@@ -8412,7 +8443,7 @@
       <c r="L44">
         <v>7</v>
       </c>
-      <c r="M44" s="1">
+      <c r="M44" s="2">
         <v>43732</v>
       </c>
     </row>
@@ -8438,7 +8469,7 @@
       <c r="L45">
         <v>7</v>
       </c>
-      <c r="M45" s="1">
+      <c r="M45" s="2">
         <v>43739</v>
       </c>
     </row>
@@ -8470,7 +8501,7 @@
       <c r="L46">
         <v>20</v>
       </c>
-      <c r="M46" s="1">
+      <c r="M46" s="2">
         <v>43746</v>
       </c>
     </row>
@@ -8496,7 +8527,7 @@
       <c r="L47">
         <v>7</v>
       </c>
-      <c r="M47" s="1">
+      <c r="M47" s="2">
         <v>43757</v>
       </c>
     </row>
@@ -8519,7 +8550,7 @@
       <c r="L48">
         <v>7</v>
       </c>
-      <c r="M48" s="1">
+      <c r="M48" s="2">
         <v>43761</v>
       </c>
     </row>
@@ -8545,7 +8576,7 @@
       <c r="L49">
         <v>7</v>
       </c>
-      <c r="M49" s="1">
+      <c r="M49" s="2">
         <v>43767</v>
       </c>
     </row>
@@ -8571,7 +8602,7 @@
       <c r="L50">
         <v>7</v>
       </c>
-      <c r="M50" s="1">
+      <c r="M50" s="2">
         <v>43774</v>
       </c>
     </row>
@@ -8597,7 +8628,7 @@
       <c r="L51">
         <v>7</v>
       </c>
-      <c r="M51" s="1">
+      <c r="M51" s="2">
         <v>43781</v>
       </c>
     </row>
@@ -8623,7 +8654,7 @@
       <c r="L52">
         <v>7</v>
       </c>
-      <c r="M52" s="1">
+      <c r="M52" s="2">
         <v>43788</v>
       </c>
     </row>
@@ -8649,7 +8680,7 @@
       <c r="L53">
         <v>7</v>
       </c>
-      <c r="M53" s="1">
+      <c r="M53" s="2">
         <v>43795</v>
       </c>
     </row>
@@ -8675,7 +8706,7 @@
       <c r="L54">
         <v>7</v>
       </c>
-      <c r="M54" s="1">
+      <c r="M54" s="2">
         <v>43802</v>
       </c>
     </row>
@@ -8707,7 +8738,7 @@
       <c r="L55">
         <v>20</v>
       </c>
-      <c r="M55" s="1">
+      <c r="M55" s="2">
         <v>43809</v>
       </c>
     </row>
@@ -8733,7 +8764,7 @@
       <c r="L56">
         <v>7</v>
       </c>
-      <c r="M56" s="1">
+      <c r="M56" s="2">
         <v>43817</v>
       </c>
     </row>
@@ -8753,7 +8784,7 @@
       <c r="L57">
         <v>7</v>
       </c>
-      <c r="M57" s="1">
+      <c r="M57" s="2">
         <v>43824</v>
       </c>
     </row>
@@ -8761,7 +8792,7 @@
       <c r="A58">
         <v>58</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>437</v>
       </c>
       <c r="C58" t="s">
@@ -8776,7 +8807,7 @@
       <c r="L58">
         <v>7</v>
       </c>
-      <c r="M58" s="1">
+      <c r="M58" s="2">
         <v>43830</v>
       </c>
     </row>
@@ -8805,7 +8836,7 @@
       <c r="L59">
         <v>11</v>
       </c>
-      <c r="M59" s="1">
+      <c r="M59" s="2">
         <v>43839</v>
       </c>
     </row>
@@ -8831,7 +8862,7 @@
       <c r="L60">
         <v>7</v>
       </c>
-      <c r="M60" s="1">
+      <c r="M60" s="2">
         <v>43846</v>
       </c>
     </row>
@@ -8857,7 +8888,7 @@
       <c r="L61">
         <v>7</v>
       </c>
-      <c r="M61" s="1">
+      <c r="M61" s="2">
         <v>43851</v>
       </c>
     </row>
@@ -8889,7 +8920,7 @@
       <c r="L62">
         <v>13</v>
       </c>
-      <c r="M62" t="s">
+      <c r="M62" s="2" t="s">
         <v>136</v>
       </c>
     </row>
@@ -8918,7 +8949,7 @@
       <c r="L63">
         <v>20</v>
       </c>
-      <c r="M63" s="1">
+      <c r="M63" s="2">
         <v>43867</v>
       </c>
     </row>
@@ -8944,7 +8975,7 @@
       <c r="L64">
         <v>7</v>
       </c>
-      <c r="M64" s="1">
+      <c r="M64" s="2">
         <v>43872</v>
       </c>
     </row>
@@ -8973,7 +9004,7 @@
       <c r="L65">
         <v>11</v>
       </c>
-      <c r="M65" s="1">
+      <c r="M65" s="2">
         <v>43881</v>
       </c>
     </row>
@@ -8999,7 +9030,7 @@
       <c r="L66">
         <v>7</v>
       </c>
-      <c r="M66" s="1">
+      <c r="M66" s="2">
         <v>43886</v>
       </c>
     </row>
@@ -9025,7 +9056,7 @@
       <c r="L67">
         <v>7</v>
       </c>
-      <c r="M67" s="1">
+      <c r="M67" s="2">
         <v>43893</v>
       </c>
     </row>
@@ -9048,7 +9079,7 @@
       <c r="L68">
         <v>7</v>
       </c>
-      <c r="M68" s="1">
+      <c r="M68" s="2">
         <v>43900</v>
       </c>
     </row>
@@ -9074,7 +9105,7 @@
       <c r="L69">
         <v>7</v>
       </c>
-      <c r="M69" s="1">
+      <c r="M69" s="2">
         <v>43909</v>
       </c>
     </row>
@@ -9094,7 +9125,7 @@
       <c r="L70">
         <v>7</v>
       </c>
-      <c r="M70" s="1">
+      <c r="M70" s="2">
         <v>43914</v>
       </c>
     </row>
@@ -9120,7 +9151,7 @@
       <c r="L71">
         <v>7</v>
       </c>
-      <c r="M71" s="1">
+      <c r="M71" s="2">
         <v>43920</v>
       </c>
     </row>
@@ -9146,7 +9177,7 @@
       <c r="L72">
         <v>7</v>
       </c>
-      <c r="M72" s="1">
+      <c r="M72" s="2">
         <v>43926</v>
       </c>
     </row>
@@ -9172,7 +9203,7 @@
       <c r="L73">
         <v>7</v>
       </c>
-      <c r="M73" s="1">
+      <c r="M73" s="2">
         <v>43929</v>
       </c>
     </row>
@@ -9198,7 +9229,7 @@
       <c r="L74">
         <v>7</v>
       </c>
-      <c r="M74" s="1">
+      <c r="M74" s="2">
         <v>43934</v>
       </c>
     </row>
@@ -9224,7 +9255,7 @@
       <c r="L75">
         <v>7</v>
       </c>
-      <c r="M75" s="1">
+      <c r="M75" s="2">
         <v>43941</v>
       </c>
     </row>
@@ -9250,7 +9281,7 @@
       <c r="L76">
         <v>7</v>
       </c>
-      <c r="M76" s="1">
+      <c r="M76" s="2">
         <v>43948</v>
       </c>
     </row>
@@ -9276,7 +9307,7 @@
       <c r="L77">
         <v>7</v>
       </c>
-      <c r="M77" s="1">
+      <c r="M77" s="2">
         <v>43955</v>
       </c>
     </row>
@@ -9302,7 +9333,7 @@
       <c r="L78">
         <v>7</v>
       </c>
-      <c r="M78" s="1">
+      <c r="M78" s="2">
         <v>43961</v>
       </c>
     </row>
@@ -9328,7 +9359,7 @@
       <c r="L79">
         <v>7</v>
       </c>
-      <c r="M79" s="1">
+      <c r="M79" s="2">
         <v>43969</v>
       </c>
     </row>
@@ -9354,7 +9385,7 @@
       <c r="L80">
         <v>7</v>
       </c>
-      <c r="M80" s="1">
+      <c r="M80" s="2">
         <v>43976</v>
       </c>
     </row>
@@ -9383,7 +9414,7 @@
       <c r="L81">
         <v>13</v>
       </c>
-      <c r="M81" s="1">
+      <c r="M81" s="2">
         <v>43984</v>
       </c>
     </row>
@@ -9409,7 +9440,7 @@
       <c r="L82">
         <v>7</v>
       </c>
-      <c r="M82" s="1">
+      <c r="M82" s="2">
         <v>43991</v>
       </c>
     </row>
@@ -9435,7 +9466,7 @@
       <c r="L83">
         <v>7</v>
       </c>
-      <c r="M83" s="1">
+      <c r="M83" s="2">
         <v>43998</v>
       </c>
     </row>
@@ -9458,7 +9489,7 @@
       <c r="L84">
         <v>18</v>
       </c>
-      <c r="M84" s="1">
+      <c r="M84" s="2">
         <v>44734</v>
       </c>
     </row>
@@ -9484,7 +9515,7 @@
       <c r="L85">
         <v>7</v>
       </c>
-      <c r="M85" s="1">
+      <c r="M85" s="2">
         <v>44013</v>
       </c>
     </row>
@@ -9510,7 +9541,7 @@
       <c r="L86">
         <v>7</v>
       </c>
-      <c r="M86" s="1">
+      <c r="M86" s="2">
         <v>44019</v>
       </c>
     </row>
@@ -9536,7 +9567,7 @@
       <c r="L87">
         <v>7</v>
       </c>
-      <c r="M87" s="1">
+      <c r="M87" s="2">
         <v>44025</v>
       </c>
     </row>
@@ -9562,7 +9593,7 @@
       <c r="L88">
         <v>7</v>
       </c>
-      <c r="M88" s="1">
+      <c r="M88" s="2">
         <v>44033</v>
       </c>
     </row>
@@ -9588,7 +9619,7 @@
       <c r="L89">
         <v>7</v>
       </c>
-      <c r="M89" s="1">
+      <c r="M89" s="2">
         <v>44041</v>
       </c>
     </row>
@@ -9614,7 +9645,7 @@
       <c r="L90">
         <v>7</v>
       </c>
-      <c r="M90" s="1">
+      <c r="M90" s="2">
         <v>44047</v>
       </c>
     </row>
@@ -9640,7 +9671,7 @@
       <c r="L91">
         <v>7</v>
       </c>
-      <c r="M91" s="1">
+      <c r="M91" s="2">
         <v>44054</v>
       </c>
     </row>
@@ -9669,7 +9700,7 @@
       <c r="L92">
         <v>13</v>
       </c>
-      <c r="M92" s="1">
+      <c r="M92" s="2">
         <v>44061</v>
       </c>
     </row>
@@ -9701,7 +9732,7 @@
       <c r="L93">
         <v>10</v>
       </c>
-      <c r="M93" s="1">
+      <c r="M93" s="2">
         <v>44073</v>
       </c>
     </row>
@@ -9733,7 +9764,7 @@
       <c r="L94">
         <v>10</v>
       </c>
-      <c r="M94" s="1">
+      <c r="M94" s="2">
         <v>44076</v>
       </c>
     </row>
@@ -9759,7 +9790,7 @@
       <c r="L95">
         <v>7</v>
       </c>
-      <c r="M95" s="1">
+      <c r="M95" s="2">
         <v>44083</v>
       </c>
     </row>
@@ -9785,7 +9816,7 @@
       <c r="L96">
         <v>7</v>
       </c>
-      <c r="M96" s="1">
+      <c r="M96" s="2">
         <v>44088</v>
       </c>
     </row>
@@ -9814,7 +9845,7 @@
       <c r="L97">
         <v>11</v>
       </c>
-      <c r="M97" s="1">
+      <c r="M97" s="2">
         <v>44095</v>
       </c>
     </row>
@@ -9840,7 +9871,7 @@
       <c r="L98">
         <v>7</v>
       </c>
-      <c r="M98" s="1">
+      <c r="M98" s="2">
         <v>44103</v>
       </c>
     </row>
@@ -9866,7 +9897,7 @@
       <c r="L99">
         <v>7</v>
       </c>
-      <c r="M99" s="1">
+      <c r="M99" s="2">
         <v>44110</v>
       </c>
     </row>
@@ -9892,7 +9923,7 @@
       <c r="L100">
         <v>7</v>
       </c>
-      <c r="M100" s="1">
+      <c r="M100" s="2">
         <v>44117</v>
       </c>
     </row>
@@ -9921,7 +9952,7 @@
       <c r="L101">
         <v>12</v>
       </c>
-      <c r="M101" s="1">
+      <c r="M101" s="2">
         <v>44124</v>
       </c>
     </row>
@@ -9947,7 +9978,7 @@
       <c r="L102">
         <v>7</v>
       </c>
-      <c r="M102" s="1">
+      <c r="M102" s="2">
         <v>44131</v>
       </c>
     </row>
@@ -9970,7 +10001,7 @@
       <c r="L103">
         <v>7</v>
       </c>
-      <c r="M103" s="1">
+      <c r="M103" s="2">
         <v>44136</v>
       </c>
     </row>
@@ -9996,7 +10027,7 @@
       <c r="L104">
         <v>7</v>
       </c>
-      <c r="M104" s="1">
+      <c r="M104" s="2">
         <v>44145</v>
       </c>
     </row>
@@ -10022,7 +10053,7 @@
       <c r="L105">
         <v>7</v>
       </c>
-      <c r="M105" s="1">
+      <c r="M105" s="2">
         <v>44152</v>
       </c>
     </row>
@@ -10054,7 +10085,7 @@
       <c r="L106">
         <v>22</v>
       </c>
-      <c r="M106" s="1">
+      <c r="M106" s="2">
         <v>44157</v>
       </c>
     </row>
@@ -10080,7 +10111,7 @@
       <c r="L107">
         <v>7</v>
       </c>
-      <c r="M107" s="1">
+      <c r="M107" s="2">
         <v>44166</v>
       </c>
     </row>
@@ -10106,7 +10137,7 @@
       <c r="L108">
         <v>7</v>
       </c>
-      <c r="M108" s="1">
+      <c r="M108" s="2">
         <v>44172</v>
       </c>
     </row>
@@ -10135,7 +10166,7 @@
       <c r="L109">
         <v>13</v>
       </c>
-      <c r="M109" s="1">
+      <c r="M109" s="2">
         <v>44180</v>
       </c>
     </row>
@@ -10161,7 +10192,7 @@
       <c r="L110">
         <v>7</v>
       </c>
-      <c r="M110" s="1">
+      <c r="M110" s="2">
         <v>44186</v>
       </c>
     </row>
@@ -10184,7 +10215,7 @@
       <c r="L111">
         <v>16</v>
       </c>
-      <c r="M111" s="1">
+      <c r="M111" s="2">
         <v>44190</v>
       </c>
     </row>
@@ -10213,7 +10244,7 @@
       <c r="L112">
         <v>11</v>
       </c>
-      <c r="M112" s="1">
+      <c r="M112" s="2">
         <v>44201</v>
       </c>
     </row>
@@ -10239,7 +10270,7 @@
       <c r="L113">
         <v>7</v>
       </c>
-      <c r="M113" s="1">
+      <c r="M113" s="2">
         <v>44208</v>
       </c>
     </row>
@@ -10265,7 +10296,7 @@
       <c r="L114">
         <v>7</v>
       </c>
-      <c r="M114" s="1">
+      <c r="M114" s="2">
         <v>44215</v>
       </c>
     </row>
@@ -10291,7 +10322,7 @@
       <c r="L115">
         <v>7</v>
       </c>
-      <c r="M115" s="1">
+      <c r="M115" s="2">
         <v>44222</v>
       </c>
     </row>
@@ -10320,7 +10351,7 @@
       <c r="L116">
         <v>11</v>
       </c>
-      <c r="M116" s="1">
+      <c r="M116" s="2">
         <v>44229</v>
       </c>
     </row>
@@ -10346,7 +10377,7 @@
       <c r="L117">
         <v>7</v>
       </c>
-      <c r="M117" s="1">
+      <c r="M117" s="2">
         <v>44236</v>
       </c>
     </row>
@@ -10378,7 +10409,7 @@
       <c r="L118">
         <v>7</v>
       </c>
-      <c r="M118" s="1">
+      <c r="M118" s="2">
         <v>44241</v>
       </c>
     </row>
@@ -10404,7 +10435,7 @@
       <c r="L119">
         <v>7</v>
       </c>
-      <c r="M119" s="1">
+      <c r="M119" s="2">
         <v>44243</v>
       </c>
     </row>
@@ -10430,7 +10461,7 @@
       <c r="L120">
         <v>7</v>
       </c>
-      <c r="M120" s="1">
+      <c r="M120" s="2">
         <v>44251</v>
       </c>
     </row>
@@ -10456,7 +10487,7 @@
       <c r="L121">
         <v>7</v>
       </c>
-      <c r="M121" s="1">
+      <c r="M121" s="2">
         <v>44257</v>
       </c>
     </row>
@@ -10482,7 +10513,7 @@
       <c r="L122">
         <v>7</v>
       </c>
-      <c r="M122" s="1">
+      <c r="M122" s="2">
         <v>44264</v>
       </c>
     </row>
@@ -10508,7 +10539,7 @@
       <c r="L123">
         <v>7</v>
       </c>
-      <c r="M123" s="1">
+      <c r="M123" s="2">
         <v>44269</v>
       </c>
     </row>
@@ -10534,7 +10565,7 @@
       <c r="L124">
         <v>7</v>
       </c>
-      <c r="M124" s="1">
+      <c r="M124" s="2">
         <v>44271</v>
       </c>
     </row>
@@ -10563,7 +10594,7 @@
       <c r="L125">
         <v>7</v>
       </c>
-      <c r="M125" s="1">
+      <c r="M125" s="2">
         <v>44278</v>
       </c>
     </row>
@@ -10589,7 +10620,7 @@
       <c r="L126">
         <v>7</v>
       </c>
-      <c r="M126" s="1">
+      <c r="M126" s="2">
         <v>44285</v>
       </c>
     </row>
@@ -10612,7 +10643,7 @@
       <c r="L127">
         <v>7</v>
       </c>
-      <c r="M127" s="1">
+      <c r="M127" s="2">
         <v>44292</v>
       </c>
     </row>
@@ -10638,7 +10669,7 @@
       <c r="L128">
         <v>7</v>
       </c>
-      <c r="M128" s="1">
+      <c r="M128" s="2">
         <v>44299</v>
       </c>
     </row>
@@ -10667,7 +10698,7 @@
       <c r="L129">
         <v>20</v>
       </c>
-      <c r="M129" s="1">
+      <c r="M129" s="2">
         <v>44307</v>
       </c>
     </row>
@@ -10693,7 +10724,7 @@
       <c r="L130">
         <v>7</v>
       </c>
-      <c r="M130" s="1">
+      <c r="M130" s="2">
         <v>44313</v>
       </c>
     </row>
@@ -10719,7 +10750,7 @@
       <c r="L131">
         <v>7</v>
       </c>
-      <c r="M131" s="1">
+      <c r="M131" s="2">
         <v>44320</v>
       </c>
     </row>
@@ -10745,7 +10776,7 @@
       <c r="L132">
         <v>7</v>
       </c>
-      <c r="M132" s="1">
+      <c r="M132" s="2">
         <v>44327</v>
       </c>
     </row>
@@ -10777,7 +10808,7 @@
       <c r="L133">
         <v>13</v>
       </c>
-      <c r="M133" s="1">
+      <c r="M133" s="2">
         <v>44334</v>
       </c>
     </row>
@@ -10803,7 +10834,7 @@
       <c r="L134">
         <v>7</v>
       </c>
-      <c r="M134" s="1">
+      <c r="M134" s="2">
         <v>44341</v>
       </c>
     </row>
@@ -10829,7 +10860,7 @@
       <c r="L135">
         <v>7</v>
       </c>
-      <c r="M135" s="1">
+      <c r="M135" s="2">
         <v>44348</v>
       </c>
     </row>
@@ -10858,7 +10889,7 @@
       <c r="L136">
         <v>13</v>
       </c>
-      <c r="M136" s="1">
+      <c r="M136" s="2">
         <v>44355</v>
       </c>
     </row>
@@ -10884,7 +10915,7 @@
       <c r="L137">
         <v>7</v>
       </c>
-      <c r="M137" s="1">
+      <c r="M137" s="2">
         <v>44362</v>
       </c>
     </row>
@@ -10910,7 +10941,7 @@
       <c r="L138">
         <v>7</v>
       </c>
-      <c r="M138" s="1">
+      <c r="M138" s="2">
         <v>44369</v>
       </c>
     </row>
@@ -10936,7 +10967,7 @@
       <c r="L139">
         <v>7</v>
       </c>
-      <c r="M139" s="1">
+      <c r="M139" s="2">
         <v>44376</v>
       </c>
     </row>
@@ -10962,7 +10993,7 @@
       <c r="L140">
         <v>7</v>
       </c>
-      <c r="M140" s="1">
+      <c r="M140" s="2">
         <v>44378</v>
       </c>
     </row>
@@ -10988,7 +11019,7 @@
       <c r="L141">
         <v>7</v>
       </c>
-      <c r="M141" s="1">
+      <c r="M141" s="2">
         <v>44390</v>
       </c>
     </row>
@@ -11014,7 +11045,7 @@
       <c r="L142">
         <v>7</v>
       </c>
-      <c r="M142" s="1">
+      <c r="M142" s="2">
         <v>44397</v>
       </c>
     </row>
@@ -11022,7 +11053,7 @@
       <c r="A143">
         <v>142</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B143" s="1" t="s">
         <v>2272</v>
       </c>
       <c r="C143" t="s">
@@ -11040,7 +11071,7 @@
       <c r="L143">
         <v>7</v>
       </c>
-      <c r="M143" s="1">
+      <c r="M143" s="2">
         <v>44404</v>
       </c>
     </row>
@@ -11066,7 +11097,7 @@
       <c r="L144">
         <v>7</v>
       </c>
-      <c r="M144" s="1">
+      <c r="M144" s="2">
         <v>44411</v>
       </c>
     </row>
@@ -11089,7 +11120,7 @@
       <c r="L145">
         <v>7</v>
       </c>
-      <c r="M145" s="1">
+      <c r="M145" s="2">
         <v>44418</v>
       </c>
     </row>
@@ -11115,7 +11146,7 @@
       <c r="L146">
         <v>7</v>
       </c>
-      <c r="M146" s="1">
+      <c r="M146" s="2">
         <v>44424</v>
       </c>
     </row>
@@ -11147,7 +11178,7 @@
       <c r="L147">
         <v>20</v>
       </c>
-      <c r="M147" s="1">
+      <c r="M147" s="2">
         <v>44431</v>
       </c>
     </row>
@@ -11173,7 +11204,7 @@
       <c r="L148">
         <v>7</v>
       </c>
-      <c r="M148" s="1">
+      <c r="M148" s="2">
         <v>44439</v>
       </c>
     </row>
@@ -11199,7 +11230,7 @@
       <c r="L149">
         <v>7</v>
       </c>
-      <c r="M149" s="1">
+      <c r="M149" s="2">
         <v>44446</v>
       </c>
     </row>
@@ -11225,7 +11256,7 @@
       <c r="L150">
         <v>7</v>
       </c>
-      <c r="M150" s="1">
+      <c r="M150" s="2">
         <v>44453</v>
       </c>
     </row>
@@ -11251,7 +11282,7 @@
       <c r="L151">
         <v>7</v>
       </c>
-      <c r="M151" s="1">
+      <c r="M151" s="2">
         <v>44461</v>
       </c>
     </row>
@@ -11277,7 +11308,7 @@
       <c r="L152">
         <v>7</v>
       </c>
-      <c r="M152" s="1">
+      <c r="M152" s="2">
         <v>44467</v>
       </c>
     </row>
@@ -11306,7 +11337,7 @@
       <c r="L153">
         <v>11</v>
       </c>
-      <c r="M153" s="1">
+      <c r="M153" s="2">
         <v>44474</v>
       </c>
     </row>
@@ -11332,7 +11363,7 @@
       <c r="L154">
         <v>7</v>
       </c>
-      <c r="M154" s="1">
+      <c r="M154" s="2">
         <v>44481</v>
       </c>
     </row>
@@ -11358,7 +11389,7 @@
       <c r="L155">
         <v>7</v>
       </c>
-      <c r="M155" s="1">
+      <c r="M155" s="2">
         <v>44487</v>
       </c>
     </row>
@@ -11387,7 +11418,7 @@
       <c r="L156">
         <v>13</v>
       </c>
-      <c r="M156" s="1">
+      <c r="M156" s="2">
         <v>44496</v>
       </c>
     </row>
@@ -11419,7 +11450,7 @@
       <c r="L157">
         <v>13</v>
       </c>
-      <c r="M157" s="1">
+      <c r="M157" s="2">
         <v>44502</v>
       </c>
     </row>
@@ -11445,7 +11476,7 @@
       <c r="L158">
         <v>7</v>
       </c>
-      <c r="M158" s="1">
+      <c r="M158" s="2">
         <v>44505</v>
       </c>
     </row>
@@ -11477,7 +11508,7 @@
       <c r="L159">
         <v>13</v>
       </c>
-      <c r="M159" s="1">
+      <c r="M159" s="2">
         <v>44510</v>
       </c>
     </row>
@@ -11503,7 +11534,7 @@
       <c r="L160">
         <v>7</v>
       </c>
-      <c r="M160" s="1">
+      <c r="M160" s="2">
         <v>44516</v>
       </c>
     </row>
@@ -11529,7 +11560,7 @@
       <c r="L161">
         <v>7</v>
       </c>
-      <c r="M161" s="1">
+      <c r="M161" s="2">
         <v>44523</v>
       </c>
     </row>
@@ -11555,7 +11586,7 @@
       <c r="L162">
         <v>7</v>
       </c>
-      <c r="M162" s="1">
+      <c r="M162" s="2">
         <v>44530</v>
       </c>
     </row>
@@ -11581,7 +11612,7 @@
       <c r="L163">
         <v>7</v>
       </c>
-      <c r="M163" s="1">
+      <c r="M163" s="2">
         <v>44538</v>
       </c>
     </row>
@@ -11607,7 +11638,7 @@
       <c r="L164">
         <v>7</v>
       </c>
-      <c r="M164" s="1">
+      <c r="M164" s="2">
         <v>44544</v>
       </c>
     </row>
@@ -11633,7 +11664,7 @@
       <c r="L165">
         <v>7</v>
       </c>
-      <c r="M165" s="1">
+      <c r="M165" s="2">
         <v>44551</v>
       </c>
     </row>
@@ -11656,7 +11687,7 @@
       <c r="L166">
         <v>7</v>
       </c>
-      <c r="M166" s="1">
+      <c r="M166" s="2">
         <v>44554</v>
       </c>
     </row>
@@ -11679,7 +11710,7 @@
       <c r="L167">
         <v>7</v>
       </c>
-      <c r="M167" s="1">
+      <c r="M167" s="2">
         <v>44565</v>
       </c>
     </row>
@@ -11705,7 +11736,7 @@
       <c r="L168">
         <v>7</v>
       </c>
-      <c r="M168" s="1">
+      <c r="M168" s="2">
         <v>44572</v>
       </c>
     </row>
@@ -11731,7 +11762,7 @@
       <c r="L169">
         <v>11</v>
       </c>
-      <c r="M169" s="1">
+      <c r="M169" s="2">
         <v>44579</v>
       </c>
     </row>
@@ -11757,7 +11788,7 @@
       <c r="L170">
         <v>7</v>
       </c>
-      <c r="M170" s="1">
+      <c r="M170" s="2">
         <v>44583</v>
       </c>
     </row>
@@ -11783,7 +11814,7 @@
       <c r="L171">
         <v>7</v>
       </c>
-      <c r="M171" s="1">
+      <c r="M171" s="2">
         <v>44586</v>
       </c>
     </row>
@@ -11809,7 +11840,7 @@
       <c r="L172">
         <v>7</v>
       </c>
-      <c r="M172" s="1">
+      <c r="M172" s="2">
         <v>44593</v>
       </c>
     </row>
@@ -11835,7 +11866,7 @@
       <c r="L173">
         <v>7</v>
       </c>
-      <c r="M173" s="1">
+      <c r="M173" s="2">
         <v>44600</v>
       </c>
     </row>
@@ -11861,7 +11892,7 @@
       <c r="L174">
         <v>7</v>
       </c>
-      <c r="M174" s="1">
+      <c r="M174" s="2">
         <v>44607</v>
       </c>
     </row>
@@ -11887,7 +11918,7 @@
       <c r="L175">
         <v>7</v>
       </c>
-      <c r="M175" s="1">
+      <c r="M175" s="2">
         <v>44614</v>
       </c>
     </row>
@@ -11919,7 +11950,7 @@
       <c r="L176">
         <v>18</v>
       </c>
-      <c r="M176" s="1">
+      <c r="M176" s="2">
         <v>44621</v>
       </c>
     </row>
@@ -11945,7 +11976,7 @@
       <c r="L177">
         <v>7</v>
       </c>
-      <c r="M177" s="1">
+      <c r="M177" s="2">
         <v>44628</v>
       </c>
     </row>
@@ -11971,7 +12002,7 @@
       <c r="L178">
         <v>7</v>
       </c>
-      <c r="M178" s="1">
+      <c r="M178" s="2">
         <v>44635</v>
       </c>
     </row>
@@ -12003,7 +12034,7 @@
       <c r="L179">
         <v>20</v>
       </c>
-      <c r="M179" s="1">
+      <c r="M179" s="2">
         <v>44642</v>
       </c>
     </row>
@@ -12029,7 +12060,7 @@
       <c r="L180">
         <v>7</v>
       </c>
-      <c r="M180" s="1">
+      <c r="M180" s="2">
         <v>44649</v>
       </c>
     </row>
@@ -12055,7 +12086,7 @@
       <c r="L181">
         <v>7</v>
       </c>
-      <c r="M181" s="1">
+      <c r="M181" s="2">
         <v>44656</v>
       </c>
     </row>
@@ -12081,7 +12112,7 @@
       <c r="L182">
         <v>7</v>
       </c>
-      <c r="M182" s="1">
+      <c r="M182" s="2">
         <v>44663</v>
       </c>
     </row>
@@ -12113,7 +12144,7 @@
       <c r="L183">
         <v>14</v>
       </c>
-      <c r="M183" s="1">
+      <c r="M183" s="2">
         <v>44670</v>
       </c>
     </row>
@@ -12139,7 +12170,7 @@
       <c r="L184">
         <v>7</v>
       </c>
-      <c r="M184" s="1">
+      <c r="M184" s="2">
         <v>44677</v>
       </c>
     </row>
@@ -12165,7 +12196,7 @@
       <c r="L185">
         <v>7</v>
       </c>
-      <c r="M185" s="1">
+      <c r="M185" s="2">
         <v>44683</v>
       </c>
     </row>
@@ -12191,7 +12222,7 @@
       <c r="L186">
         <v>7</v>
       </c>
-      <c r="M186" s="1">
+      <c r="M186" s="2">
         <v>44690</v>
       </c>
     </row>
@@ -12217,7 +12248,7 @@
       <c r="L187">
         <v>7</v>
       </c>
-      <c r="M187" s="1">
+      <c r="M187" s="2">
         <v>44697</v>
       </c>
     </row>
@@ -12249,7 +12280,7 @@
       <c r="L188">
         <v>13</v>
       </c>
-      <c r="M188" s="1">
+      <c r="M188" s="2">
         <v>44704</v>
       </c>
     </row>
@@ -12275,7 +12306,7 @@
       <c r="L189">
         <v>7</v>
       </c>
-      <c r="M189" s="1">
+      <c r="M189" s="2">
         <v>44711</v>
       </c>
     </row>
@@ -12301,7 +12332,7 @@
       <c r="L190">
         <v>7</v>
       </c>
-      <c r="M190" s="1">
+      <c r="M190" s="2">
         <v>44718</v>
       </c>
     </row>
@@ -12327,7 +12358,7 @@
       <c r="L191">
         <v>7</v>
       </c>
-      <c r="M191" s="1">
+      <c r="M191" s="2">
         <v>44725</v>
       </c>
     </row>
@@ -12359,7 +12390,7 @@
       <c r="L192">
         <v>21</v>
       </c>
-      <c r="M192" s="1">
+      <c r="M192" s="2">
         <v>44732</v>
       </c>
     </row>
@@ -12385,7 +12416,7 @@
       <c r="L193">
         <v>7</v>
       </c>
-      <c r="M193" s="1">
+      <c r="M193" s="2">
         <v>44739</v>
       </c>
     </row>
@@ -12411,7 +12442,7 @@
       <c r="L194">
         <v>7</v>
       </c>
-      <c r="M194" s="1">
+      <c r="M194" s="2">
         <v>44747</v>
       </c>
     </row>
@@ -12437,7 +12468,7 @@
       <c r="L195">
         <v>7</v>
       </c>
-      <c r="M195" s="1">
+      <c r="M195" s="2">
         <v>44753</v>
       </c>
     </row>
@@ -12463,7 +12494,7 @@
       <c r="L196">
         <v>7</v>
       </c>
-      <c r="M196" s="1">
+      <c r="M196" s="2">
         <v>44760</v>
       </c>
     </row>
@@ -12495,7 +12526,7 @@
       <c r="L197">
         <v>12</v>
       </c>
-      <c r="M197" s="1">
+      <c r="M197" s="2">
         <v>44767</v>
       </c>
     </row>
@@ -12521,7 +12552,7 @@
       <c r="L198">
         <v>7</v>
       </c>
-      <c r="M198" s="1">
+      <c r="M198" s="2">
         <v>44774</v>
       </c>
     </row>
@@ -12550,7 +12581,7 @@
       <c r="L199">
         <v>11</v>
       </c>
-      <c r="M199" s="1">
+      <c r="M199" s="2">
         <v>44781</v>
       </c>
     </row>
@@ -12579,7 +12610,7 @@
       <c r="L200">
         <v>7</v>
       </c>
-      <c r="M200" s="1">
+      <c r="M200" s="2">
         <v>44788</v>
       </c>
     </row>
@@ -12605,7 +12636,7 @@
       <c r="L201">
         <v>7</v>
       </c>
-      <c r="M201" s="1">
+      <c r="M201" s="2">
         <v>44802</v>
       </c>
     </row>
@@ -12628,7 +12659,7 @@
       <c r="L202">
         <v>7</v>
       </c>
-      <c r="M202" s="1">
+      <c r="M202" s="2">
         <v>44810</v>
       </c>
     </row>
@@ -12657,7 +12688,7 @@
       <c r="L203">
         <v>13</v>
       </c>
-      <c r="M203" s="1">
+      <c r="M203" s="2">
         <v>44816</v>
       </c>
     </row>
@@ -12683,7 +12714,7 @@
       <c r="L204">
         <v>7</v>
       </c>
-      <c r="M204" s="1">
+      <c r="M204" s="2">
         <v>44823</v>
       </c>
     </row>
@@ -12709,7 +12740,7 @@
       <c r="L205">
         <v>7</v>
       </c>
-      <c r="M205" s="1">
+      <c r="M205" s="2">
         <v>44831</v>
       </c>
     </row>
@@ -12735,7 +12766,7 @@
       <c r="L206">
         <v>7</v>
       </c>
-      <c r="M206" s="1">
+      <c r="M206" s="2">
         <v>44837</v>
       </c>
     </row>
@@ -12764,7 +12795,7 @@
       <c r="L207">
         <v>11</v>
       </c>
-      <c r="M207" s="1">
+      <c r="M207" s="2">
         <v>44844</v>
       </c>
     </row>
@@ -12790,7 +12821,7 @@
       <c r="L208">
         <v>7</v>
       </c>
-      <c r="M208" s="1">
+      <c r="M208" s="2">
         <v>44851</v>
       </c>
     </row>
@@ -12819,7 +12850,7 @@
       <c r="L209">
         <v>13</v>
       </c>
-      <c r="M209" s="1">
+      <c r="M209" s="2">
         <v>44865</v>
       </c>
     </row>
@@ -12845,7 +12876,7 @@
       <c r="L210">
         <v>7</v>
       </c>
-      <c r="M210" s="1">
+      <c r="M210" s="2">
         <v>44872</v>
       </c>
     </row>
@@ -12871,7 +12902,7 @@
       <c r="L211">
         <v>7</v>
       </c>
-      <c r="M211" s="1">
+      <c r="M211" s="2">
         <v>44879</v>
       </c>
     </row>
@@ -12900,7 +12931,7 @@
       <c r="L212">
         <v>11</v>
       </c>
-      <c r="M212" s="1">
+      <c r="M212" s="2">
         <v>44886</v>
       </c>
     </row>
@@ -12932,7 +12963,7 @@
       <c r="L213">
         <v>16</v>
       </c>
-      <c r="M213" s="1">
+      <c r="M213" s="2">
         <v>44893</v>
       </c>
     </row>
@@ -12961,7 +12992,7 @@
       <c r="L214">
         <v>13</v>
       </c>
-      <c r="M214" s="1">
+      <c r="M214" s="2">
         <v>44900</v>
       </c>
     </row>
@@ -12987,7 +13018,7 @@
       <c r="L215">
         <v>7</v>
       </c>
-      <c r="M215" s="1">
+      <c r="M215" s="2">
         <v>44907</v>
       </c>
     </row>
@@ -13013,7 +13044,7 @@
       <c r="L216">
         <v>7</v>
       </c>
-      <c r="M216" s="1">
+      <c r="M216" s="2">
         <v>44914</v>
       </c>
     </row>
@@ -13033,7 +13064,7 @@
       <c r="L217">
         <v>7</v>
       </c>
-      <c r="M217" s="1">
+      <c r="M217" s="2">
         <v>44919</v>
       </c>
     </row>
@@ -13062,7 +13093,7 @@
       <c r="L218">
         <v>11</v>
       </c>
-      <c r="M218" s="1">
+      <c r="M218" s="2">
         <v>44928</v>
       </c>
     </row>
@@ -13097,7 +13128,7 @@
       <c r="L219">
         <v>10</v>
       </c>
-      <c r="M219" s="1">
+      <c r="M219" s="2">
         <v>44936</v>
       </c>
     </row>
@@ -13129,7 +13160,7 @@
       <c r="L220">
         <v>12</v>
       </c>
-      <c r="M220" s="1">
+      <c r="M220" s="2">
         <v>44943</v>
       </c>
     </row>
@@ -13164,7 +13195,7 @@
       <c r="L221">
         <v>10</v>
       </c>
-      <c r="M221" s="1">
+      <c r="M221" s="2">
         <v>44950</v>
       </c>
     </row>
@@ -13193,7 +13224,7 @@
       <c r="L222">
         <v>11</v>
       </c>
-      <c r="M222" s="1">
+      <c r="M222" s="2">
         <v>44957</v>
       </c>
     </row>
@@ -13219,7 +13250,7 @@
       <c r="L223">
         <v>7</v>
       </c>
-      <c r="M223" s="1">
+      <c r="M223" s="2">
         <v>44963</v>
       </c>
     </row>
@@ -13245,7 +13276,7 @@
       <c r="L224">
         <v>7</v>
       </c>
-      <c r="M224" s="1">
+      <c r="M224" s="2">
         <v>44970</v>
       </c>
     </row>
@@ -13271,7 +13302,7 @@
       <c r="L225">
         <v>7</v>
       </c>
-      <c r="M225" s="1">
+      <c r="M225" s="2">
         <v>44977</v>
       </c>
     </row>
@@ -13297,7 +13328,7 @@
       <c r="L226">
         <v>7</v>
       </c>
-      <c r="M226" s="1">
+      <c r="M226" s="2">
         <v>44984</v>
       </c>
     </row>
@@ -13326,7 +13357,7 @@
       <c r="L227">
         <v>20</v>
       </c>
-      <c r="M227" s="1">
+      <c r="M227" s="2">
         <v>44991</v>
       </c>
     </row>
@@ -13352,7 +13383,7 @@
       <c r="L228">
         <v>7</v>
       </c>
-      <c r="M228" s="1">
+      <c r="M228" s="2">
         <v>44998</v>
       </c>
     </row>
@@ -13378,7 +13409,7 @@
       <c r="L229">
         <v>7</v>
       </c>
-      <c r="M229" s="1">
+      <c r="M229" s="2">
         <v>45005</v>
       </c>
     </row>
@@ -13404,7 +13435,7 @@
       <c r="L230">
         <v>7</v>
       </c>
-      <c r="M230" s="1">
+      <c r="M230" s="2">
         <v>45012</v>
       </c>
     </row>
@@ -13433,7 +13464,7 @@
       <c r="L231">
         <v>9</v>
       </c>
-      <c r="M231" s="1">
+      <c r="M231" s="2">
         <v>45019</v>
       </c>
     </row>
@@ -13459,7 +13490,7 @@
       <c r="L232">
         <v>7</v>
       </c>
-      <c r="M232" s="1">
+      <c r="M232" s="2">
         <v>45026</v>
       </c>
     </row>
@@ -13485,8 +13516,8 @@
       <c r="L233">
         <v>7</v>
       </c>
-      <c r="M233" s="3">
-        <v>45017</v>
+      <c r="M233" s="2">
+        <v>45033</v>
       </c>
     </row>
     <row r="234" spans="1:13" x14ac:dyDescent="0.25">
@@ -13514,8 +13545,8 @@
       <c r="L234">
         <v>11</v>
       </c>
-      <c r="M234" s="3">
-        <v>45017</v>
+      <c r="M234" s="2">
+        <v>45041</v>
       </c>
     </row>
     <row r="235" spans="1:13" x14ac:dyDescent="0.25">
@@ -13540,8 +13571,8 @@
       <c r="L235">
         <v>7</v>
       </c>
-      <c r="M235" s="3">
-        <v>45047</v>
+      <c r="M235" s="2">
+        <v>45054</v>
       </c>
     </row>
     <row r="236" spans="1:13" x14ac:dyDescent="0.25">
@@ -13566,7 +13597,7 @@
       <c r="L236">
         <v>7</v>
       </c>
-      <c r="M236" s="3">
+      <c r="M236" s="2">
         <v>45047</v>
       </c>
     </row>
@@ -13595,8 +13626,8 @@
       <c r="L237">
         <v>13</v>
       </c>
-      <c r="M237" s="3">
-        <v>45047</v>
+      <c r="M237" s="2">
+        <v>45061</v>
       </c>
     </row>
     <row r="238" spans="1:13" x14ac:dyDescent="0.25">
@@ -13621,7 +13652,7 @@
       <c r="L238">
         <v>7</v>
       </c>
-      <c r="M238" s="3">
+      <c r="M238" s="2">
         <v>45047</v>
       </c>
     </row>
@@ -13647,8 +13678,8 @@
       <c r="L239">
         <v>7</v>
       </c>
-      <c r="M239" s="3">
-        <v>45047</v>
+      <c r="M239" s="2">
+        <v>45068</v>
       </c>
     </row>
     <row r="240" spans="1:13" x14ac:dyDescent="0.25">
@@ -13656,28 +13687,216 @@
         <v>235</v>
       </c>
       <c r="B240" t="s">
+        <v>2292</v>
+      </c>
+      <c r="C240" t="s">
+        <v>211</v>
+      </c>
+      <c r="D240" t="s">
+        <v>61</v>
+      </c>
+      <c r="I240" t="s">
+        <v>6</v>
+      </c>
+      <c r="J240" t="s">
+        <v>7</v>
+      </c>
+      <c r="L240">
+        <v>7</v>
+      </c>
+      <c r="M240" s="2">
+        <v>45082</v>
+      </c>
+    </row>
+    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>236</v>
+      </c>
+      <c r="B241" t="s">
+        <v>2293</v>
+      </c>
+      <c r="C241" t="s">
+        <v>129</v>
+      </c>
+      <c r="D241" t="s">
+        <v>173</v>
+      </c>
+      <c r="I241" t="s">
+        <v>6</v>
+      </c>
+      <c r="J241" t="s">
+        <v>214</v>
+      </c>
+      <c r="L241">
+        <v>7</v>
+      </c>
+      <c r="M241" s="2">
+        <v>45089</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>237</v>
+      </c>
+      <c r="B242" t="s">
         <v>2289</v>
       </c>
-      <c r="C240" t="s">
+      <c r="C242" t="s">
         <v>2290</v>
       </c>
-      <c r="D240" t="s">
+      <c r="D242" t="s">
         <v>161</v>
       </c>
-      <c r="E240" t="s">
+      <c r="E242" t="s">
         <v>79</v>
       </c>
-      <c r="I240" t="s">
-        <v>6</v>
-      </c>
-      <c r="J240" t="s">
-        <v>7</v>
-      </c>
-      <c r="L240">
+      <c r="I242" t="s">
+        <v>6</v>
+      </c>
+      <c r="J242" t="s">
+        <v>7</v>
+      </c>
+      <c r="L242">
         <v>13</v>
       </c>
-      <c r="M240" s="3">
-        <v>45108</v>
+      <c r="M242" s="2">
+        <v>45103</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>238</v>
+      </c>
+      <c r="B243" t="s">
+        <v>2294</v>
+      </c>
+      <c r="C243" t="s">
+        <v>7</v>
+      </c>
+      <c r="D243" t="s">
+        <v>135</v>
+      </c>
+      <c r="E243" t="s">
+        <v>15</v>
+      </c>
+      <c r="I243" t="s">
+        <v>6</v>
+      </c>
+      <c r="L243">
+        <v>9</v>
+      </c>
+      <c r="M243" s="2">
+        <v>45110</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>239</v>
+      </c>
+      <c r="B244" t="s">
+        <v>2295</v>
+      </c>
+      <c r="C244" t="s">
+        <v>22</v>
+      </c>
+      <c r="D244" t="s">
+        <v>77</v>
+      </c>
+      <c r="E244" t="s">
+        <v>79</v>
+      </c>
+      <c r="H244" t="s">
+        <v>2296</v>
+      </c>
+      <c r="I244" t="s">
+        <v>6</v>
+      </c>
+      <c r="J244" t="s">
+        <v>7</v>
+      </c>
+      <c r="L244">
+        <v>11</v>
+      </c>
+      <c r="M244" s="2">
+        <v>45118</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>240</v>
+      </c>
+      <c r="B245" t="s">
+        <v>2297</v>
+      </c>
+      <c r="C245" t="s">
+        <v>2277</v>
+      </c>
+      <c r="D245" t="s">
+        <v>251</v>
+      </c>
+      <c r="I245" t="s">
+        <v>6</v>
+      </c>
+      <c r="J245" t="s">
+        <v>7</v>
+      </c>
+      <c r="L245">
+        <v>7</v>
+      </c>
+      <c r="M245" s="2">
+        <v>45124</v>
+      </c>
+    </row>
+    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>241</v>
+      </c>
+      <c r="B246" t="s">
+        <v>2298</v>
+      </c>
+      <c r="C246" t="s">
+        <v>2286</v>
+      </c>
+      <c r="D246" t="s">
+        <v>2287</v>
+      </c>
+      <c r="I246" t="s">
+        <v>6</v>
+      </c>
+      <c r="J246" t="s">
+        <v>7</v>
+      </c>
+      <c r="L246">
+        <v>7</v>
+      </c>
+      <c r="M246" s="2">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>242</v>
+      </c>
+      <c r="B247" t="s">
+        <v>2299</v>
+      </c>
+      <c r="C247" t="s">
+        <v>25</v>
+      </c>
+      <c r="D247" t="s">
+        <v>4</v>
+      </c>
+      <c r="I247" t="s">
+        <v>6</v>
+      </c>
+      <c r="J247" t="s">
+        <v>7</v>
+      </c>
+      <c r="L247">
+        <v>7</v>
+      </c>
+      <c r="M247" s="2">
+        <v>45138</v>
       </c>
     </row>
   </sheetData>
@@ -13687,6 +13906,153 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B1BA6E-3B38-48FD-9DE6-F99BA09A07E6}">
+  <dimension ref="A1:A25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2291</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A492">
+    <sortCondition ref="A1:A492"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43091EBA-A0D4-4432-83DD-E76C36865AD9}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A1835"/>
@@ -13726,7 +14092,7 @@
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>637</v>
       </c>
     </row>
@@ -22882,4 +23248,1050 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0A5748-C4FE-4E84-8B72-3469EDDDACD0}">
+  <dimension ref="A1:C978"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>2284</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>2277</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>2282</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>2275</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>2287</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>2279</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="978" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C978" t="s">
+        <v>2296</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A978">
+    <sortCondition ref="A1:A978"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>